<commit_message>
Re-factor of tableau structure
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/MutableTableauTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/MutableTableauTest.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="construct 3x5" sheetId="1" r:id="rId1"/>
     <sheet name="construct aux 4x6" sheetId="2" r:id="rId2"/>
     <sheet name="swap 2,3" sheetId="4" r:id="rId3"/>
-    <sheet name="swap aux 5,0" sheetId="5" r:id="rId4"/>
+    <sheet name="swap aux 0,5" sheetId="5" r:id="rId4"/>
     <sheet name="swap aux 3,9 1,3" sheetId="6" r:id="rId5"/>
     <sheet name="rand" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
   <si>
     <t>#0</t>
   </si>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H30" sqref="A29:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,6 +1253,57 @@
       </c>
       <c r="H31" s="6">
         <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="H35">
+        <v>7</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+      <c r="J35">
+        <v>9</v>
+      </c>
+      <c r="K35">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1754,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,7 +2702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
@@ -3306,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="B46">
-        <f t="shared" ref="B46:J46" si="16">B42</f>
+        <f t="shared" ref="B46:H46" si="16">B42</f>
         <v>1</v>
       </c>
       <c r="C46">
@@ -3733,1251 +3784,1251 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*20-7</f>
-        <v>-6.2160798163761726</v>
+        <v>9.4974891305704396</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:L16" ca="1" si="0">RAND()*20-7</f>
-        <v>-2.7515430970568815</v>
+        <v>12.508023831331521</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8412978612548443</v>
+        <v>-1.0184303246218462</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.778595704795912</v>
+        <v>-4.1392257660054508</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.671538874940484</v>
+        <v>7.8392954820175547</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8498799556440808</v>
+        <v>-6.2262093511807475</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.30043481110808123</v>
+        <v>2.0195308020009684</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.2169174774565432</v>
+        <v>-4.8091367174940167</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7353550594659639</v>
+        <v>5.757642434550986</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3981975894809366</v>
+        <v>-0.66026633526639333</v>
       </c>
       <c r="K1">
         <f ca="1">RAND()*20-7</f>
-        <v>1.560991933509424</v>
+        <v>2.816958269532055</v>
       </c>
       <c r="L1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2837233872999505</v>
+        <v>2.6230764641563518</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:L25" ca="1" si="1">RAND()*20-7</f>
-        <v>10.202303718767247</v>
+        <v>5.7388734042680323</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.397463804062113</v>
+        <v>-1.2452206210200316</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8524731806546999</v>
+        <v>-6.3002180592872215</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>12.972390829925743</v>
+        <v>-4.268416699456659</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.6108823276922113</v>
+        <v>1.9849318416415116</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5757659112709099</v>
+        <v>12.063763112077822</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1832245910740582</v>
+        <v>6.039472002965411</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.090551987772832</v>
+        <v>-5.2735274080289063</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6599590882920054</v>
+        <v>6.2441483027328992</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6783539148926714</v>
+        <v>4.7233308035698904</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1546410142939614</v>
+        <v>5.7781612946073722</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.9876785913763921</v>
+        <v>3.0603683463057365</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.5405321869682957</v>
+        <v>4.135019216937641</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.3004118712888264</v>
+        <v>-5.9807303909008969</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>10.283206100520012</v>
+        <v>1.8289521238051343</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2295987781094766</v>
+        <v>-4.5367386081397969</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3229756102028354</v>
+        <v>12.704973872432905</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10219897568136105</v>
+        <v>0.30141031722320033</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9897055960918841</v>
+        <v>12.817562601188442</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>11.429080436060115</v>
+        <v>2.9845770722839831</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5406798840768907</v>
+        <v>-6.6551317255862923</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.1226241759603255</v>
+        <v>-2.7669158004158056</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2822884763212379</v>
+        <v>0.23721453405956794</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9444667287342199</v>
+        <v>4.3104828722128854</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0975560304762393</v>
+        <v>3.6999294970864689</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7029798566128083</v>
+        <v>6.8742180748029824</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.204927125210947</v>
+        <v>7.0389563233189385</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.0181701147190769</v>
+        <v>5.1280016712675405</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2079356347735484</v>
+        <v>1.0437891437225328</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.2399586626661101</v>
+        <v>10.009354082799256</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.01878943171128</v>
+        <v>2.9375068630819268</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1650466969063995</v>
+        <v>-3.9512294314826883</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8739713809509553</v>
+        <v>6.6965988632651445</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.5467649443004179</v>
+        <v>-4.7525324969243297</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3831957958730214</v>
+        <v>4.8650794497385252</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4153056384472755</v>
+        <v>3.4553271425891197</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.3522438262928675</v>
+        <v>5.7925956514599442</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>10.044753165329855</v>
+        <v>1.0906168061323527</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1461020828333801</v>
+        <v>4.6242703686709916</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4666771427612186</v>
+        <v>3.5549799330636258</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0343882834429046</v>
+        <v>-3.3551515354382593</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2993377018449124</v>
+        <v>0.52998793473525119</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0785760547749952</v>
+        <v>-2.4869464048435717</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5356933441546534</v>
+        <v>8.3726343379945298</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1800835217731276</v>
+        <v>-6.7032326667125179</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3414797158770639</v>
+        <v>11.915003475334661</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.241466800724039</v>
+        <v>5.9629248508514578</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>12.587650864073051</v>
+        <v>4.052673878690003</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6847451366919231E-2</v>
+        <v>-0.84317774834864068</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.4190246652907246</v>
+        <v>0.40611291360393498</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2854561743607462</v>
+        <v>2.9896082404745847</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9253697289801934</v>
+        <v>-0.48988270476650264</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.969997396154227</v>
+        <v>7.0585117326560862</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0196696509447527</v>
+        <v>-2.2061128151658558</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>12.095108869235801</v>
+        <v>7.8718844335323208</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.8667117380467975</v>
+        <v>11.66677237091308</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8595338559671042</v>
+        <v>-1.6597677534553839</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4601588143934539</v>
+        <v>-4.4484372087835542</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9281302451113493</v>
+        <v>6.9014738163538283</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0204047140252186</v>
+        <v>4.2408416756258731</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>11.427946913911978</v>
+        <v>12.716185744913993</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7015131583362688</v>
+        <v>10.933622899608782</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1679675712727313</v>
+        <v>0.10605138488470178</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.9385735126923418</v>
+        <v>-0.28527925439894908</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4408497800549505</v>
+        <v>-2.3563423701513768</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>12.196796670696155</v>
+        <v>7.5034356861578413</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7745473953781143</v>
+        <v>-6.0540855890727601</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5478735639894374</v>
+        <v>1.1958081275634687</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.049654227959909</v>
+        <v>-6.1759168823611281</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6075748524703819</v>
+        <v>-4.0920074622681124</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.286250270675538</v>
+        <v>12.786562682810715</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53226073887305336</v>
+        <v>-2.9972464444636531</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3534891794476493</v>
+        <v>-0.88865146589083821</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1822659981833255</v>
+        <v>3.2897821114633956</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.1378380646967088</v>
+        <v>-3.3756293449231149</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.4801344645146521</v>
+        <v>-4.8875534209721891</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>12.139602829872537</v>
+        <v>3.5412745438838584</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9727994502165362</v>
+        <v>9.5762974465647588</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>12.256181118699615</v>
+        <v>2.5381856010362149</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>10.450055099708376</v>
+        <v>12.617537615985732</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.26604301708649025</v>
+        <v>3.5527238577435014</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2261319862676423</v>
+        <v>11.982508314601169</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7810900523999482</v>
+        <v>2.9221870836725685</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7780639678064318</v>
+        <v>12.463852784939363</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6437036896110477</v>
+        <v>6.2678186461966732</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3524456368595335</v>
+        <v>5.46723881547757</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2489054657482797</v>
+        <v>12.741881179441609</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.7999149535058709</v>
+        <v>1.035703605450788</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.91327012225495</v>
+        <v>-1.8340839950245629</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7334376493855981</v>
+        <v>10.345060458270076</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>10.340740958956992</v>
+        <v>4.1662996129609216</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.6529473947314646</v>
+        <v>9.4218588399694312</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.9385687475308275</v>
+        <v>12.71198667918728</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3962554952069137</v>
+        <v>2.0851589604368215</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>11.036887041508137</v>
+        <v>2.3954913153108865</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.196778339910419</v>
+        <v>8.4080210892046807</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2157903386870679</v>
+        <v>5.8995770622458146</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>12.951237436359289</v>
+        <v>9.9591984925874186</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7955991389888837</v>
+        <v>5.6290956235287606</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9642911087586459</v>
+        <v>0.63424545289074441</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>12.276816842994837</v>
+        <v>4.7314314114448788</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>5.769851650584501</v>
+        <v>-1.7682336186269758</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.5116678627508202</v>
+        <v>-3.9696568463720432</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28703876374484594</v>
+        <v>8.7479843654672784</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.3194874084313533</v>
+        <v>12.561225201914375</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0942081600995461</v>
+        <v>-4.8214973304061601</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5175864815923568</v>
+        <v>3.5490924909503754</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6318778216870129</v>
+        <v>-5.9128782931142947</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0875526724084317</v>
+        <v>-2.1149501669265867</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.30099342543577912</v>
+        <v>6.6841302885302785</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8282117697207045</v>
+        <v>12.041938945309127</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>12.67540522916158</v>
+        <v>11.61207697758157</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6756352532694336</v>
+        <v>3.4397387712756551</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5963206074586083</v>
+        <v>-1.0810636522553363</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1563469117150511</v>
+        <v>1.986403087655388</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5448233368996078</v>
+        <v>11.233619574580484</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8143327375939791</v>
+        <v>0.6422274158864445</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0414530677665113</v>
+        <v>6.7453858230707997</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82147632136859006</v>
+        <v>-5.2139829923237322</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.5084558998924735</v>
+        <v>8.3078455490330949</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.1402970594688053</v>
+        <v>-2.541398244487981</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4893988538257688</v>
+        <v>-5.375008942583646</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2227588020821241</v>
+        <v>8.5674835320689571</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7952992996925907</v>
+        <v>8.403481805424569</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.198092166513888</v>
+        <v>4.400215603334253</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3855927446294949</v>
+        <v>8.5518619735911283</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1250036021529475</v>
+        <v>8.8701729253656705</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.6432568307727768</v>
+        <v>-4.1110047558794909</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>11.354413183505319</v>
+        <v>0.80191461397468267</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.770753246118709</v>
+        <v>4.5705808727796562</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6440619671034824</v>
+        <v>-5.0557848140837862</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2235192770557788</v>
+        <v>1.9491213656519886</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.2304507973936101</v>
+        <v>8.6709032498394585</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8904702344336162</v>
+        <v>-1.0019989624895942</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>12.575279877295877</v>
+        <v>7.8122021670420896</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.9331863294618499</v>
+        <v>1.4132048554611387</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7738500489895621</v>
+        <v>5.1235994052703653</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4191077360837774</v>
+        <v>1.1740660644592005</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6221762472079835</v>
+        <v>8.8368792295081366</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.0571126779940272E-2</v>
+        <v>9.7820874153396034</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7779906161363277</v>
+        <v>11.341170570847048</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96174748446747493</v>
+        <v>-5.1795118970760132</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7186216092114144</v>
+        <v>-3.2209220315355451</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.9494251907568776</v>
+        <v>6.2308371711746844</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16804866572717536</v>
+        <v>0.84224060110897181</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>12.487637710930105</v>
+        <v>11.242871984624387</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8065130324746157</v>
+        <v>1.5223419745176638</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6629399610832376</v>
+        <v>2.685535023447569</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.3847463412471521</v>
+        <v>-4.2686529374954372</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8327086681268447</v>
+        <v>3.2577872108640484</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.077370709025967</v>
+        <v>2.009427147946699</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24658059188763737</v>
+        <v>12.884636609096066</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.097199846990792</v>
+        <v>4.7642999707202023</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1747548740520362</v>
+        <v>10.112061376349345</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7105045261400953</v>
+        <v>3.9131535034916105</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4439635536789162</v>
+        <v>9.3985269793221526E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>2.908497565584808</v>
+        <v>12.7749848623939</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2491090560538609</v>
+        <v>-2.2162730378639033</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8214172186603097</v>
+        <v>-6.8269081142997461</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5262626569218476</v>
+        <v>5.8260507891354294</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.8437878083222525</v>
+        <v>5.8604315813162113</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.68124731951337214</v>
+        <v>11.613396288621097</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.9221086035213752</v>
+        <v>2.1244000888190655</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>12.381316996027639</v>
+        <v>-5.0796213645515031</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.9383765757255054</v>
+        <v>6.4815380443589721</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72953617100484003</v>
+        <v>11.393029743484814</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0195720417563727</v>
+        <v>5.8800590607560661</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="0"/>
-        <v>9.1282731141137177</v>
+        <v>-2.4171511590807686</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3139282919199733</v>
+        <v>-3.0801692720179634</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7825669984715304</v>
+        <v>12.65854410625197</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1804930082279057</v>
+        <v>8.6312976919941455</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.118231645064288</v>
+        <v>6.3330692276408964</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.6815391591075999</v>
+        <v>-2.5906683373170214</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>12.712638445789207</v>
+        <v>-4.8164402639445552</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>11.903116154669952</v>
+        <v>-2.9773446575184348</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8104594268806711</v>
+        <v>1.5190904414607154</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3819968909487343</v>
+        <v>-3.5378942345936442</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.5377159258169004</v>
+        <v>2.1127107042492881</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4995820377829254</v>
+        <v>10.812861244529348</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6241886124691902</v>
+        <v>10.263807297766068</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.6956180235445002</v>
+        <v>11.155015769042731</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>11.545231793764373</v>
+        <v>0.65134102764616131</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1915862934861323</v>
+        <v>4.1002483793499724</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.4217001283161439</v>
+        <v>11.209867624574144</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.9468844609710407</v>
+        <v>0.10520984716650261</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6498285897770799</v>
+        <v>6.4824288217632642E-2</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8162647034547987</v>
+        <v>8.9712313688806677</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1644488930067567</v>
+        <v>4.6629259205322313</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.7586978718890522</v>
+        <v>4.852159884079164</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>11.906599202259621</v>
+        <v>1.2832284530832894</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>10.508583841513484</v>
+        <v>0.30081362264334732</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.836292974448213</v>
+        <v>10.203378921314211</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3617513202931981</v>
+        <v>8.7392553388377561</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>12.676174782580127</v>
+        <v>-3.7906064620048423</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7303548718059112E-2</v>
+        <v>3.4809738487742763</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5548109997138386</v>
+        <v>9.745750455543579</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8226741878587553</v>
+        <v>-4.1873752146640246</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8422924626013959</v>
+        <v>-4.0752397584913158</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5687697789248194</v>
+        <v>2.8956824570075383</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.8277806288893377</v>
+        <v>-4.6802806523009775</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3401054918529862</v>
+        <v>12.529363627469547</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.43367773587411662</v>
+        <v>9.2946982978796129</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>9.658615535006188</v>
+        <v>2.0484662876118911</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35557172055842656</v>
+        <v>-4.4206276405768445</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2683273320300614</v>
+        <v>4.2791360658784434</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6051823695814154</v>
+        <v>12.804857311408345</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.7558768481768681</v>
+        <v>0.21055297440837784</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3103631615955464</v>
+        <v>11.334037713101555</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.9636316867611932</v>
+        <v>-5.8517952136519167</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.9483321635558521</v>
+        <v>-4.6315922354213424</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>10.32304053051007</v>
+        <v>2.0383976127753094</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9387524967331569</v>
+        <v>3.8357815276578009</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.0648541454921023</v>
+        <v>9.3035851175501065</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2953401883585993</v>
+        <v>2.5268850819393229</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.0175177926304713</v>
+        <v>9.0209675883335052</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5208921497118268</v>
+        <v>3.3808463391950099</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>11.651298343762313</v>
+        <v>8.8411584298167973</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.4034514798421704</v>
+        <v>12.851650741027658</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0177777410878299</v>
+        <v>-2.6501824359627806</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6474697151295317</v>
+        <v>-5.1620745299452242</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1577427871722179</v>
+        <v>8.1507388814013684</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.4297367135795334</v>
+        <v>1.7506862474078346</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.85571390878776832</v>
+        <v>6.0807226982376879</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2811947531115813</v>
+        <v>4.464204729882832</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.3898916904193541</v>
+        <v>11.62700527211376</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.56078991199550554</v>
+        <v>-5.9394369193387231</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6555113464060831</v>
+        <v>1.7507160754535889</v>
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="1"/>
-        <v>12.064249009771942</v>
+        <v>8.8042765020169753</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.0754953614999496</v>
+        <v>-6.6759604653676901</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9372942706528793</v>
+        <v>-4.7863840421265813</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>10.241133502161922</v>
+        <v>5.6190187094038038</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.2383475809046223</v>
+        <v>10.11906619516434</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5418281846256363</v>
+        <v>7.1986283568548011</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>10.073997667666575</v>
+        <v>-0.2401489114899924</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>11.464203316856295</v>
+        <v>11.942924823673611</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2209845946474633</v>
+        <v>10.29853956543095</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6883941843684429</v>
+        <v>12.629829919024793</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0138960649397379</v>
+        <v>-2.5437389152357568</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.721778999356129</v>
+        <v>-0.98734671605045943</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.3894334648121678</v>
+        <v>11.766452008241483</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.5778300362310258</v>
+        <v>1.637440234541117</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7962649924357308</v>
+        <v>-2.6298932494201193</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.71792532498924899</v>
+        <v>2.9685381470515324</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8325823256177323</v>
+        <v>4.6997650627760859</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>8.601013251609837</v>
+        <v>-4.5408166722956</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7960218256380713</v>
+        <v>2.2143562215482504</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>9.7977535750009963</v>
+        <v>-4.7784053055605762</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.4345093977615182</v>
+        <v>10.351392631685176</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9101057584870116</v>
+        <v>7.0442103470227515</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>9.6228836855202786</v>
+        <v>-0.90160433773718829</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8560091649831101</v>
+        <v>2.5582436906377399</v>
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3224641030479702</v>
+        <v>-2.3046270744437329</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8895772051798936</v>
+        <v>-4.8526326896640324</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3597823706789161</v>
+        <v>11.75805633266576</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4427702946242018</v>
+        <v>-5.4027883272614741</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.5052212153620399</v>
+        <v>-0.14900664434694555</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.48054040655205732</v>
+        <v>3.7930392121173782</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6123763191646461</v>
+        <v>4.6995266608838566</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.3960267029800955</v>
+        <v>6.7150415088227824</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.659259865898906</v>
+        <v>-0.72565714598701359</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.2206835556049356</v>
+        <v>7.2224794965458621</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.9249836202454986</v>
+        <v>11.12013434658045</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.1566359681712051</v>
+        <v>-3.2516881374304445</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7406857238951545</v>
+        <v>-0.98519171745570233</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5593499667412107</v>
+        <v>-2.7367317899071502</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>10.973344870936948</v>
+        <v>11.687339604783759</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.2461689252093713</v>
+        <v>10.588562768759665</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3927579973151367</v>
+        <v>-6.8056749596439818</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>11.855174508605515</v>
+        <v>-0.33035942656805251</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.2145376346921903</v>
+        <v>6.97651436910024</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97223406907809906</v>
+        <v>5.9797499335403792</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8537404324988955</v>
+        <v>11.226337498910262</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1048692332469265</v>
+        <v>-5.4043854543126217</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.8320641571361573</v>
+        <v>0.97126726714625988</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
-        <v>7.103594237047691</v>
+        <v>7.2979211129824044</v>
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.7336230176646295</v>
+        <v>8.4935939133387244</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.0782707547875923</v>
+        <v>-0.77471663994238593</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>3.402972210807512</v>
+        <v>5.8330072559913777</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3704356534596425</v>
+        <v>-3.4179972799229601</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.8244822996211107</v>
+        <v>-1.061805515874843</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70998194785560642</v>
+        <v>3.58064670776821</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.1099786095656707</v>
+        <v>10.586477849920463</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.32398865551405898</v>
+        <v>-5.5809420556921108</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>10.055661395445597</v>
+        <v>10.44079654375621</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>9.6463088837430533</v>
+        <v>8.6398819028502025</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2553923905140962</v>
+        <v>8.1037086471474407</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6189901580699111</v>
+        <v>-1.765690141660059</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.2042067006415245</v>
+        <v>12.850999686381329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>